<commit_message>
Add Rev 4/5 control separation and comparison data
- Create r4_r5_comparison.json from NIST comparison workbook
  - 90 withdrawn controls (Rev 4 only)
  - 268 new controls (Rev 5 only)
- Update script to separate Rev 4-only controls into dedicated sheet
  - Rev 5 controls stay in level sheets
  - Rev 4-only (withdrawn) controls go to orange-highlighted sheet
  - Loads Rev 4 reference data for withdrawn controls
- Add sp800-53r4-to-r5-comparison-workbook.xlsx source file
- Update CLAUDE.md with new structure and features
</commit_message>
<xml_diff>
--- a/level_data_CCI_Breakdown.xlsx
+++ b/level_data_CCI_Breakdown.xlsx
@@ -1538,7 +1538,7 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Authorization and Permissions</t>
+          <t>Authority and Purpose</t>
         </is>
       </c>
       <c r="C16" s="4" t="n">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Authorization and Permissions</t>
+          <t>Authority and Purpose</t>
         </is>
       </c>
       <c r="C25" s="4" t="n">

</xml_diff>

<commit_message>
Filter out empty families and Unknown from Rev 5 summary
- Summary tables now only show families with actual controls (>0 total)
- Exclude "Unknown" family from summary charts and tables
- Updated table titles to indicate "Rev 5" data
- Level sheets continue to only show Rev 5 controls
- Rev 4-only controls remain isolated in separate sheet
</commit_message>
<xml_diff>
--- a/level_data_CCI_Breakdown.xlsx
+++ b/level_data_CCI_Breakdown.xlsx
@@ -1446,7 +1446,7 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Controls by Family Across Levels</t>
+          <t>Controls by Family Across Levels (Rev 5)</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CCI Count by Family Across Levels</t>
+          <t>CCI Count by Family Across Levels (Rev 5)</t>
         </is>
       </c>
     </row>

</xml_diff>